<commit_message>
Update 221007_VPS 1팀 마일스톤_V110.xlsx
</commit_message>
<xml_diff>
--- a/일정관리/221007_VPS 1팀 마일스톤_V110.xlsx
+++ b/일정관리/221007_VPS 1팀 마일스톤_V110.xlsx
@@ -1339,535 +1339,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>캐릭터</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>컨셉</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">스토리
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>세부</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">취향
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>호감도</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">시스템
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>상황</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>별</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">대사
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>플레이어</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>만보기</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">연동
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>코인</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>재화</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">)
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">인벤토리
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>데이트</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>시스템</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>사진</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">&amp; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>다이어리</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">컨텐츠
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>돌발</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">이벤트
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>선물</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>구매</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>&amp;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">선물
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>UI
-Sound Effect</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>기능 최적화
 최종 빌드 구현</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1979,6 +1450,535 @@
         <charset val="129"/>
       </rPr>
       <t>완성</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>캐릭터</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>컨셉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">스토리
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>세부</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">취향
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>호감도</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">시스템
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>상황</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>별</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">대사
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>플레이어</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>만보기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">연동
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>코인</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>재화</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">)
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">인벤토리
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>데이트</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시스템</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>사진</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>다이어리</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">컨텐츠
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>돌발</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">이벤트
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>선물</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>구매</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">선물
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>UI
+Sound Effect</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2222,6 +2222,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2255,36 +2279,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -2298,9 +2301,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -3152,8 +3152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3164,29 +3164,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="9"/>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="10" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10" t="s">
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
       <c r="M2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="9"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
@@ -3222,76 +3222,76 @@
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="13"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="21"/>
     </row>
     <row r="5" spans="2:13" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="27"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="24"/>
     </row>
     <row r="6" spans="2:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="20"/>
+      <c r="D6" s="11"/>
       <c r="E6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="22"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="35" t="s">
+      <c r="G6" s="29"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="30"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="M6" s="23"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" s="13"/>
     </row>
     <row r="7" spans="2:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="27"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="7"/>
       <c r="D7" s="8"/>
       <c r="E7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="24"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="26"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="15"/>
     </row>
     <row r="8" spans="2:13" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
@@ -3334,28 +3334,23 @@
       <c r="E9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="29"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="29"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="28" t="s">
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="M9" s="20"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M9" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="L6:M7"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="C9:D9"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="E2:H2"/>
@@ -3367,6 +3362,11 @@
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="F6:H7"/>
     <mergeCell ref="I6:K7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="L6:M7"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="C9:D9"/>
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="F8:G8"/>
   </mergeCells>

</xml_diff>